<commit_message>
update jpa + template + generate
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/QPP021_E3.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/QPP021_E3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="7740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="3780"/>
   </bookViews>
   <sheets>
     <sheet name="圧着式（はがき）サンプル" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>その他</t>
     <rPh sb="2" eb="3">
@@ -61,17 +61,7 @@
     <t>社員:</t>
   </si>
   <si>
-    <t>NNNNNNNNNNNNNNNNNNNN</t>
-  </si>
-  <si>
-    <t>NNNNNNNNNNNNNNNNNNNNNN</t>
-  </si>
-  <si>
     <t>備考</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNNN
-</t>
   </si>
   <si>
     <t>〒　999-9999</t>
@@ -120,7 +110,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,13 +183,6 @@
       <charset val="128"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="IPA明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="IPA明朝"/>
@@ -488,15 +471,9 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -518,6 +495,54 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -527,53 +552,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -860,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -869,7 +852,7 @@
     <col min="1" max="1" width="39.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="2.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="0.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" style="1" customWidth="1"/>
@@ -890,28 +873,24 @@
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="6"/>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="37"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="44"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="41"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
@@ -921,24 +900,20 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="21">
-        <v>43040</v>
-      </c>
-      <c r="E2" s="27" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="25" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="7"/>
-      <c r="G2" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="39"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="47"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="44"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
@@ -951,26 +926,26 @@
         <v>3</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="32"/>
+      <c r="D4" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="46"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="32"/>
+      <c r="G4" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="46"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="33"/>
-      <c r="L4" s="32"/>
+      <c r="J4" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="47"/>
+      <c r="L4" s="46"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="31" t="s">
+      <c r="N4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="O4" s="32"/>
+      <c r="O4" s="46"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
@@ -980,17 +955,17 @@
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="25"/>
+      <c r="D5" s="23"/>
       <c r="E5" s="16"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="25"/>
+      <c r="G5" s="23"/>
       <c r="H5" s="10"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="35"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="30"/>
       <c r="L5" s="10"/>
       <c r="M5" s="9"/>
-      <c r="N5" s="25"/>
+      <c r="N5" s="23"/>
       <c r="O5" s="18"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
@@ -1001,17 +976,17 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="25"/>
+      <c r="D6" s="23"/>
       <c r="E6" s="16"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="25"/>
+      <c r="G6" s="23"/>
       <c r="H6" s="10"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="35"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="30"/>
       <c r="L6" s="10"/>
       <c r="M6" s="9"/>
-      <c r="N6" s="25"/>
+      <c r="N6" s="23"/>
       <c r="O6" s="18"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
@@ -1022,17 +997,17 @@
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="25"/>
+      <c r="D7" s="23"/>
       <c r="E7" s="16"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="25"/>
+      <c r="G7" s="23"/>
       <c r="H7" s="10"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="35"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="30"/>
       <c r="L7" s="10"/>
       <c r="M7" s="9"/>
-      <c r="N7" s="25"/>
+      <c r="N7" s="23"/>
       <c r="O7" s="19"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
@@ -1043,17 +1018,17 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="25"/>
+      <c r="D8" s="23"/>
       <c r="E8" s="16"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="25"/>
+      <c r="G8" s="23"/>
       <c r="H8" s="10"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="35"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="30"/>
       <c r="L8" s="10"/>
       <c r="M8" s="9"/>
-      <c r="N8" s="25"/>
+      <c r="N8" s="23"/>
       <c r="O8" s="18"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -1064,17 +1039,17 @@
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="25"/>
+      <c r="D9" s="23"/>
       <c r="E9" s="16"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="25"/>
+      <c r="G9" s="23"/>
       <c r="H9" s="10"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="35"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="30"/>
       <c r="L9" s="10"/>
       <c r="M9" s="9"/>
-      <c r="N9" s="25"/>
+      <c r="N9" s="23"/>
       <c r="O9" s="18"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
@@ -1085,17 +1060,17 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="25"/>
+      <c r="D10" s="23"/>
       <c r="E10" s="16"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="25"/>
+      <c r="G10" s="23"/>
       <c r="H10" s="10"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="35"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="30"/>
       <c r="L10" s="10"/>
       <c r="M10" s="9"/>
-      <c r="N10" s="25"/>
+      <c r="N10" s="23"/>
       <c r="O10" s="18"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
@@ -1106,17 +1081,17 @@
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="25"/>
+      <c r="D11" s="23"/>
       <c r="E11" s="16"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="25"/>
+      <c r="G11" s="23"/>
       <c r="H11" s="10"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="35"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="30"/>
       <c r="L11" s="10"/>
       <c r="M11" s="9"/>
-      <c r="N11" s="26"/>
+      <c r="N11" s="24"/>
       <c r="O11" s="13"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
@@ -1127,14 +1102,14 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="25"/>
+      <c r="D12" s="23"/>
       <c r="E12" s="16"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="25"/>
+      <c r="G12" s="23"/>
       <c r="H12" s="10"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="35"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="30"/>
       <c r="L12" s="10"/>
       <c r="M12" s="9"/>
       <c r="N12" s="8"/>
@@ -1146,24 +1121,24 @@
     </row>
     <row r="13" spans="1:22" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="25"/>
+      <c r="D13" s="23"/>
       <c r="E13" s="16"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="25"/>
+      <c r="G13" s="23"/>
       <c r="H13" s="10"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="35"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="30"/>
       <c r="L13" s="10"/>
       <c r="M13" s="9"/>
-      <c r="N13" s="31" t="s">
+      <c r="N13" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="O13" s="32"/>
+      <c r="O13" s="46"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
@@ -1171,21 +1146,21 @@
     </row>
     <row r="14" spans="1:22" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="25"/>
+      <c r="D14" s="23"/>
       <c r="E14" s="16"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="25"/>
+      <c r="G14" s="23"/>
       <c r="H14" s="10"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="35"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="30"/>
       <c r="L14" s="10"/>
       <c r="M14" s="9"/>
-      <c r="N14" s="25"/>
+      <c r="N14" s="23"/>
       <c r="O14" s="18"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
@@ -1196,17 +1171,17 @@
       <c r="A15" s="4"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="25"/>
+      <c r="D15" s="23"/>
       <c r="E15" s="16"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="25"/>
+      <c r="G15" s="23"/>
       <c r="H15" s="10"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="35"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="30"/>
       <c r="L15" s="10"/>
       <c r="M15" s="9"/>
-      <c r="N15" s="25"/>
+      <c r="N15" s="23"/>
       <c r="O15" s="18"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
@@ -1214,22 +1189,22 @@
       <c r="S15"/>
     </row>
     <row r="16" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A16" s="29" t="s">
-        <v>12</v>
+      <c r="A16" s="27" t="s">
+        <v>9</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="25"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="16"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="25"/>
+      <c r="G16" s="23"/>
       <c r="H16" s="10"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="35"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="30"/>
       <c r="L16" s="10"/>
       <c r="M16" s="9"/>
-      <c r="N16" s="25"/>
+      <c r="N16" s="23"/>
       <c r="O16" s="18"/>
       <c r="V16"/>
     </row>
@@ -1237,86 +1212,86 @@
       <c r="A17" s="4"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="25"/>
+      <c r="D17" s="23"/>
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="25"/>
+      <c r="G17" s="23"/>
       <c r="H17" s="10"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="35"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="30"/>
       <c r="L17" s="10"/>
       <c r="M17" s="9"/>
-      <c r="N17" s="25"/>
+      <c r="N17" s="23"/>
       <c r="O17" s="18"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A18" s="29" t="s">
-        <v>13</v>
+      <c r="A18" s="27" t="s">
+        <v>10</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="25"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="16"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="25"/>
+      <c r="G18" s="23"/>
       <c r="H18" s="10"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="35"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="30"/>
       <c r="L18" s="10"/>
       <c r="M18" s="9"/>
-      <c r="N18" s="25"/>
+      <c r="N18" s="23"/>
       <c r="O18" s="18"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="25"/>
+      <c r="D19" s="23"/>
       <c r="E19" s="16"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="25"/>
+      <c r="G19" s="23"/>
       <c r="H19" s="10"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="35"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="30"/>
       <c r="L19" s="10"/>
       <c r="M19" s="9"/>
-      <c r="N19" s="25"/>
+      <c r="N19" s="23"/>
       <c r="O19" s="18"/>
     </row>
     <row r="20" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="25"/>
+      <c r="D20" s="23"/>
       <c r="E20" s="16"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="25"/>
+      <c r="G20" s="23"/>
       <c r="H20" s="10"/>
       <c r="I20" s="3"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="35"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="30"/>
       <c r="L20" s="10"/>
       <c r="M20" s="9"/>
-      <c r="N20" s="25"/>
+      <c r="N20" s="23"/>
       <c r="O20" s="18"/>
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A21" s="30" t="s">
-        <v>14</v>
+      <c r="A21" s="28" t="s">
+        <v>11</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="25"/>
+      <c r="D21" s="23"/>
       <c r="E21" s="16"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="25"/>
+      <c r="G21" s="23"/>
       <c r="H21" s="10"/>
       <c r="I21" s="3"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="35"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="30"/>
       <c r="L21" s="10"/>
       <c r="M21" s="9"/>
       <c r="N21" s="12"/>
@@ -1326,14 +1301,14 @@
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="25"/>
+      <c r="D22" s="23"/>
       <c r="E22" s="16"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="25"/>
+      <c r="G22" s="23"/>
       <c r="H22" s="10"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="35"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="30"/>
       <c r="L22" s="10"/>
       <c r="M22" s="9"/>
       <c r="N22" s="8"/>
@@ -1342,237 +1317,213 @@
     <row r="23" spans="1:15" ht="15.75" customHeight="1">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="25"/>
+      <c r="D23" s="23"/>
       <c r="E23" s="16"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="25"/>
+      <c r="G23" s="23"/>
       <c r="H23" s="10"/>
       <c r="I23" s="3"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="35"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="30"/>
       <c r="L23" s="10"/>
       <c r="M23" s="9"/>
-      <c r="N23" s="31" t="s">
+      <c r="N23" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="O23" s="32"/>
+      <c r="O23" s="46"/>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="25"/>
+      <c r="D24" s="23"/>
       <c r="E24" s="16"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="25"/>
+      <c r="G24" s="23"/>
       <c r="H24" s="10"/>
       <c r="I24" s="3"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="35"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="30"/>
       <c r="L24" s="10"/>
       <c r="M24" s="9"/>
-      <c r="N24" s="25"/>
+      <c r="N24" s="23"/>
       <c r="O24" s="10"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="25"/>
+      <c r="D25" s="23"/>
       <c r="E25" s="16"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="25"/>
+      <c r="G25" s="23"/>
       <c r="H25" s="10"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="35"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="30"/>
       <c r="L25" s="10"/>
       <c r="M25" s="9"/>
-      <c r="N25" s="25"/>
-      <c r="O25" s="24"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="22"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="25"/>
+      <c r="D26" s="23"/>
       <c r="E26" s="16"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="25"/>
+      <c r="G26" s="23"/>
       <c r="H26" s="10"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="35"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="30"/>
       <c r="L26" s="10"/>
       <c r="M26" s="9"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="24"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="22"/>
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="25"/>
+      <c r="D27" s="23"/>
       <c r="E27" s="16"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="25"/>
+      <c r="G27" s="23"/>
       <c r="H27" s="10"/>
       <c r="I27" s="3"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="35"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="30"/>
       <c r="L27" s="10"/>
       <c r="M27" s="9"/>
-      <c r="N27" s="25"/>
+      <c r="N27" s="23"/>
       <c r="O27" s="15"/>
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="25"/>
+      <c r="D28" s="23"/>
       <c r="E28" s="16"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="25"/>
+      <c r="G28" s="23"/>
       <c r="H28" s="10"/>
       <c r="I28" s="3"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="35"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="30"/>
       <c r="L28" s="10"/>
       <c r="M28" s="9"/>
-      <c r="N28" s="25"/>
+      <c r="N28" s="23"/>
       <c r="O28" s="11"/>
     </row>
     <row r="29" spans="1:15" ht="15.75" customHeight="1">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="25"/>
+      <c r="D29" s="23"/>
       <c r="E29" s="16"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="25"/>
+      <c r="G29" s="23"/>
       <c r="H29" s="10"/>
       <c r="I29" s="3"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="35"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="30"/>
       <c r="L29" s="10"/>
       <c r="M29" s="9"/>
-      <c r="N29" s="25"/>
+      <c r="N29" s="23"/>
       <c r="O29" s="11"/>
     </row>
     <row r="30" spans="1:15" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="25"/>
+      <c r="D30" s="23"/>
       <c r="E30" s="16"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="25"/>
+      <c r="G30" s="23"/>
       <c r="H30" s="10"/>
       <c r="I30" s="3"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="35"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="30"/>
       <c r="L30" s="10"/>
       <c r="M30" s="9"/>
-      <c r="N30" s="25"/>
+      <c r="N30" s="23"/>
       <c r="O30" s="11"/>
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="25"/>
+      <c r="D31" s="23"/>
       <c r="E31" s="16"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="25"/>
+      <c r="G31" s="23"/>
       <c r="H31" s="10"/>
       <c r="I31" s="3"/>
-      <c r="J31" s="34"/>
-      <c r="K31" s="35"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="30"/>
       <c r="L31" s="10"/>
       <c r="M31" s="9"/>
-      <c r="N31" s="25"/>
+      <c r="N31" s="23"/>
       <c r="O31" s="18"/>
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1">
       <c r="A32" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="25"/>
+        <v>13</v>
+      </c>
+      <c r="D32" s="23"/>
       <c r="E32" s="16"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="25"/>
+      <c r="G32" s="23"/>
       <c r="H32" s="10"/>
       <c r="I32" s="3"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="35"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="30"/>
       <c r="L32" s="10"/>
       <c r="M32" s="9"/>
-      <c r="N32" s="25"/>
+      <c r="N32" s="23"/>
       <c r="O32" s="18"/>
     </row>
     <row r="33" spans="1:15" ht="15.75" customHeight="1">
       <c r="A33" s="5"/>
-      <c r="D33" s="25"/>
+      <c r="D33" s="23"/>
       <c r="E33" s="16"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="25"/>
+      <c r="G33" s="23"/>
       <c r="H33" s="10"/>
       <c r="I33" s="3"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="35"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="30"/>
       <c r="L33" s="10"/>
       <c r="M33" s="9"/>
-      <c r="N33" s="25"/>
+      <c r="N33" s="23"/>
       <c r="O33" s="18"/>
     </row>
     <row r="34" spans="1:15" ht="15.75" customHeight="1">
       <c r="A34" s="2"/>
-      <c r="B34" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="26"/>
+      <c r="B34" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="24"/>
       <c r="E34" s="17"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="26"/>
+      <c r="G34" s="24"/>
       <c r="H34" s="20"/>
       <c r="I34" s="3"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="49"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="32"/>
       <c r="L34" s="20"/>
       <c r="M34" s="9"/>
-      <c r="N34" s="26"/>
+      <c r="N34" s="24"/>
       <c r="O34" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:O2"/>
-    <mergeCell ref="J5:K5"/>
     <mergeCell ref="N23:O23"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="G4:H4"/>
@@ -1589,6 +1540,30 @@
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="J15:K15"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:O2"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J30:K30"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>